<commit_message>
corrijo archivo cambio NA por 0
</commit_message>
<xml_diff>
--- a/boot/initial/data/DATOS/PELAGO/results-ANE-PEL24.xlsx
+++ b/boot/initial/data/DATOS/PELAGO/results-ANE-PEL24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/BOQUERON/BENCHMARK_2024/SS3_ane27.9a_benchmark/boot/initial/data/GADGET/DATOS_MJZ/PELAGO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/BOQUERON/BENCHMARK_2024/Review_data_available/boot/initial/data/DATOS/PELAGO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85287003-E454-0A48-9434-E6EFD0E7087A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB9E220-9D92-ED4F-9B9D-D292DA1A2285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17380" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35460" yWindow="-900" windowWidth="29400" windowHeight="17380" tabRatio="991" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="algarve+cadiz" sheetId="1" r:id="rId1"/>
@@ -530,18 +530,6 @@
   <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -551,16 +539,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -647,6 +629,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -985,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE41" sqref="AE41"/>
+    <sheetView tabSelected="1" topLeftCell="I17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1004,30 +1004,30 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="5" t="s">
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="AF1">
         <v>2.3914000000000001E-3</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="AH1">
         <v>3.4183086999999999</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1043,78 +1043,78 @@
         <f>Alg!C2+Cad!C2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="4">
         <v>2</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="4">
         <v>3</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="4">
         <v>1</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="4">
         <v>2</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="4">
         <v>3</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="8">
+      <c r="S2" s="4">
         <v>1</v>
       </c>
-      <c r="T2" s="8">
+      <c r="T2" s="4">
         <v>2</v>
       </c>
-      <c r="U2" s="8">
+      <c r="U2" s="4">
         <v>3</v>
       </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="X2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="12">
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="7">
         <v>1</v>
       </c>
-      <c r="AA2" s="12">
+      <c r="AA2" s="7">
         <v>2</v>
       </c>
-      <c r="AB2" s="13">
+      <c r="AB2" s="8">
         <v>3</v>
       </c>
-      <c r="AC2" s="14"/>
-      <c r="AE2" s="15" t="s">
+      <c r="AC2" s="54"/>
+      <c r="AE2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="AF2" s="16">
+      <c r="AF2" s="10">
         <v>2.8331050697043372E-3</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AG2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="AH2" s="16">
+      <c r="AH2" s="10">
         <v>3.4061849999999998</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AI2" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1130,83 +1130,83 @@
         <f>Alg!C3+Cad!C3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="12">
         <v>5.5</v>
       </c>
-      <c r="G3" s="19">
-        <v>0</v>
-      </c>
-      <c r="H3" s="19">
-        <v>0</v>
-      </c>
-      <c r="I3" s="19">
-        <v>0</v>
-      </c>
-      <c r="J3" s="20">
+      <c r="G3" s="13">
+        <v>0</v>
+      </c>
+      <c r="H3" s="13">
+        <v>0</v>
+      </c>
+      <c r="I3" s="13">
+        <v>0</v>
+      </c>
+      <c r="J3" s="14">
         <f>+SUM(G3:I3)</f>
         <v>0</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="12">
         <v>5.5</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="13">
         <f>+IF($J3&gt;0,G3/$J3,0)</f>
         <v>0</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="13">
         <f t="shared" ref="N3:P18" si="0">+IF($J3&gt;0,H3/$J3,0)</f>
         <v>0</v>
       </c>
-      <c r="O3" s="19">
+      <c r="O3" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P3" s="19">
+      <c r="P3" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q3" s="21">
+      <c r="Q3" s="15">
         <v>5.75</v>
       </c>
-      <c r="R3" s="22">
+      <c r="R3" s="16">
         <v>5.5</v>
       </c>
-      <c r="S3" s="19">
+      <c r="S3" s="13">
         <f>+$B3*M3</f>
         <v>0</v>
       </c>
-      <c r="T3" s="19">
+      <c r="T3" s="13">
         <f t="shared" ref="T3:V18" si="1">+$B3*N3</f>
         <v>0</v>
       </c>
-      <c r="U3" s="19">
+      <c r="U3" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V3" s="19">
+      <c r="V3" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X3" s="23">
+      <c r="X3" s="17">
         <f>$AF$2*((Y3)^$AH$2)</f>
         <v>0.94205220137192158</v>
       </c>
-      <c r="Y3" s="24">
+      <c r="Y3" s="18">
         <v>5.5</v>
       </c>
-      <c r="Z3" s="25">
+      <c r="Z3" s="19">
         <f>+S3*$X3</f>
         <v>0</v>
       </c>
-      <c r="AA3" s="26">
+      <c r="AA3" s="20">
         <f t="shared" ref="AA3:AC18" si="2">+T3*$X3</f>
         <v>0</v>
       </c>
-      <c r="AB3" s="26">
+      <c r="AB3" s="20">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC3" s="27">
+      <c r="AC3" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1223,72 +1223,72 @@
         <f>Alg!C4+Cad!C4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="12">
         <v>6</v>
       </c>
-      <c r="G4" s="19">
-        <v>0</v>
-      </c>
-      <c r="H4" s="19">
-        <v>0</v>
-      </c>
-      <c r="I4" s="19">
-        <v>0</v>
-      </c>
-      <c r="J4" s="20">
+      <c r="G4" s="13">
+        <v>0</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0</v>
+      </c>
+      <c r="I4" s="13">
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
         <f t="shared" ref="J4:J40" si="3">+SUM(G4:I4)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="12">
         <v>6</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="13">
         <f t="shared" ref="M4:P41" si="4">+IF($J4&gt;0,G4/$J4,0)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P4" s="19">
+      <c r="P4" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q4" s="21">
+      <c r="Q4" s="15">
         <f t="shared" ref="Q4" si="5">+Q3+0.5</f>
         <v>6.25</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="16">
         <v>6</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="13">
         <f t="shared" ref="S4:V40" si="6">+$B4*M4</f>
         <v>0</v>
       </c>
-      <c r="T4" s="19">
+      <c r="T4" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U4" s="19">
+      <c r="U4" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V4" s="19">
+      <c r="V4" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X4" s="23">
+      <c r="X4" s="17">
         <f t="shared" ref="X4:X40" si="7">$AF$2*((Y4)^$AH$2)</f>
         <v>1.2670384607746847</v>
       </c>
-      <c r="Y4" s="24">
+      <c r="Y4" s="18">
         <v>6</v>
       </c>
-      <c r="Z4" s="28">
+      <c r="Z4" s="22">
         <f t="shared" ref="Z4:AC40" si="8">+S4*$X4</f>
         <v>0</v>
       </c>
@@ -1300,7 +1300,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC4" s="29">
+      <c r="AC4" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1317,71 +1317,71 @@
         <f>Alg!C5+Cad!C5</f>
         <v>0</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="12">
         <v>6.5</v>
       </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="19">
-        <v>0</v>
-      </c>
-      <c r="I5" s="19">
-        <v>0</v>
-      </c>
-      <c r="J5" s="20">
+      <c r="G5" s="13">
+        <v>0</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>0</v>
+      </c>
+      <c r="J5" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="12">
         <v>6.5</v>
       </c>
-      <c r="M5" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="19">
+      <c r="M5" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P5" s="19">
+      <c r="P5" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="15">
         <v>6.75</v>
       </c>
-      <c r="R5" s="22">
+      <c r="R5" s="16">
         <v>6.5</v>
       </c>
-      <c r="S5" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T5" s="19">
+      <c r="S5" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U5" s="19">
+      <c r="U5" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V5" s="19">
+      <c r="V5" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X5" s="23">
+      <c r="X5" s="17">
         <f t="shared" si="7"/>
         <v>1.6641633870245225</v>
       </c>
-      <c r="Y5" s="24">
+      <c r="Y5" s="18">
         <v>6.5</v>
       </c>
-      <c r="Z5" s="28">
+      <c r="Z5" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -1393,7 +1393,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC5" s="29">
+      <c r="AC5" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1410,72 +1410,72 @@
         <f>Alg!C6+Cad!C6</f>
         <v>136.768234070608</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="12">
         <v>7</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="13">
         <v>1</v>
       </c>
-      <c r="H6" s="19">
-        <v>0</v>
-      </c>
-      <c r="I6" s="19">
-        <v>0</v>
-      </c>
-      <c r="J6" s="20">
+      <c r="H6" s="13">
+        <v>0</v>
+      </c>
+      <c r="I6" s="13">
+        <v>0</v>
+      </c>
+      <c r="J6" s="14">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="12">
         <v>7</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N6" s="19">
+      <c r="N6" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P6" s="19">
+      <c r="P6" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="15">
         <f t="shared" ref="Q6" si="9">+Q5+0.5</f>
         <v>7.25</v>
       </c>
-      <c r="R6" s="22">
+      <c r="R6" s="16">
         <v>7</v>
       </c>
-      <c r="S6" s="19">
+      <c r="S6" s="13">
         <f t="shared" si="6"/>
         <v>55160.655632214504</v>
       </c>
-      <c r="T6" s="19">
+      <c r="T6" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U6" s="19">
+      <c r="U6" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V6" s="19">
+      <c r="V6" s="13">
         <f t="shared" si="1"/>
         <v>55160.655632214504</v>
       </c>
-      <c r="X6" s="23">
+      <c r="X6" s="17">
         <f t="shared" si="7"/>
         <v>2.1420171746275334</v>
       </c>
-      <c r="Y6" s="24">
+      <c r="Y6" s="18">
         <v>7</v>
       </c>
-      <c r="Z6" s="28">
+      <c r="Z6" s="22">
         <f t="shared" si="8"/>
         <v>118155.07172791845</v>
       </c>
@@ -1487,7 +1487,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC6" s="29">
+      <c r="AC6" s="23">
         <f t="shared" si="2"/>
         <v>118155.07172791845</v>
       </c>
@@ -1504,71 +1504,71 @@
         <f>Alg!C7+Cad!C7</f>
         <v>378.19117874173935</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="12">
         <v>7.5</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="13">
         <v>9</v>
       </c>
-      <c r="H7" s="19">
-        <v>0</v>
-      </c>
-      <c r="I7" s="19">
-        <v>0</v>
-      </c>
-      <c r="J7" s="20">
+      <c r="H7" s="13">
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
+        <v>0</v>
+      </c>
+      <c r="J7" s="14">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="12">
         <v>7.5</v>
       </c>
-      <c r="M7" s="19">
+      <c r="M7" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P7" s="19">
+      <c r="P7" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="15">
         <v>7.75</v>
       </c>
-      <c r="R7" s="22">
+      <c r="R7" s="16">
         <v>7.5</v>
       </c>
-      <c r="S7" s="19">
+      <c r="S7" s="13">
         <f t="shared" si="6"/>
         <v>124995.14645674764</v>
       </c>
-      <c r="T7" s="19">
+      <c r="T7" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U7" s="19">
+      <c r="U7" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V7" s="19">
+      <c r="V7" s="13">
         <f t="shared" si="1"/>
         <v>124995.14645674764</v>
       </c>
-      <c r="X7" s="23">
+      <c r="X7" s="17">
         <f t="shared" si="7"/>
         <v>2.7094630371679336</v>
       </c>
-      <c r="Y7" s="24">
+      <c r="Y7" s="18">
         <v>7.5</v>
       </c>
-      <c r="Z7" s="28">
+      <c r="Z7" s="22">
         <f t="shared" si="8"/>
         <v>338669.72914995014</v>
       </c>
@@ -1580,7 +1580,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC7" s="29">
+      <c r="AC7" s="23">
         <f t="shared" si="2"/>
         <v>338669.72914995014</v>
       </c>
@@ -1597,72 +1597,72 @@
         <f>Alg!C8+Cad!C8</f>
         <v>1317.0721707911523</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="12">
         <v>8</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="13">
         <v>12</v>
       </c>
-      <c r="H8" s="19">
-        <v>0</v>
-      </c>
-      <c r="I8" s="19">
-        <v>0</v>
-      </c>
-      <c r="J8" s="20">
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="14">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="12">
         <v>8</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O8" s="19">
+      <c r="O8" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P8" s="19">
+      <c r="P8" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="15">
         <f t="shared" ref="Q8" si="10">+Q7+0.5</f>
         <v>8.25</v>
       </c>
-      <c r="R8" s="22">
+      <c r="R8" s="16">
         <v>8</v>
       </c>
-      <c r="S8" s="19">
+      <c r="S8" s="13">
         <f t="shared" si="6"/>
         <v>361190.60350257793</v>
       </c>
-      <c r="T8" s="19">
+      <c r="T8" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U8" s="19">
+      <c r="U8" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V8" s="19">
+      <c r="V8" s="13">
         <f t="shared" si="1"/>
         <v>361190.60350257793</v>
       </c>
-      <c r="X8" s="23">
+      <c r="X8" s="17">
         <f t="shared" si="7"/>
         <v>3.3756254194165338</v>
       </c>
-      <c r="Y8" s="24">
+      <c r="Y8" s="18">
         <v>8</v>
       </c>
-      <c r="Z8" s="28">
+      <c r="Z8" s="22">
         <f t="shared" si="8"/>
         <v>1219244.1824377007</v>
       </c>
@@ -1674,7 +1674,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC8" s="29">
+      <c r="AC8" s="23">
         <f t="shared" si="2"/>
         <v>1219244.1824377007</v>
       </c>
@@ -1692,71 +1692,71 @@
         <v>1872.5305217989726</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="F9" s="18">
+      <c r="F9" s="12">
         <v>8.5</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="13">
         <v>15</v>
       </c>
-      <c r="H9" s="19">
-        <v>0</v>
-      </c>
-      <c r="I9" s="19">
-        <v>0</v>
-      </c>
-      <c r="J9" s="20">
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <v>0</v>
+      </c>
+      <c r="J9" s="14">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="12">
         <v>8.5</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N9" s="19">
+      <c r="N9" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O9" s="19">
+      <c r="O9" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P9" s="19">
+      <c r="P9" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q9" s="21">
+      <c r="Q9" s="15">
         <v>8.75</v>
       </c>
-      <c r="R9" s="22">
+      <c r="R9" s="16">
         <v>8.5</v>
       </c>
-      <c r="S9" s="19">
+      <c r="S9" s="13">
         <f>+$B9*M9</f>
         <v>430796.00057672348</v>
       </c>
-      <c r="T9" s="19">
+      <c r="T9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U9" s="19">
+      <c r="U9" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V9" s="19">
+      <c r="V9" s="13">
         <f t="shared" si="1"/>
         <v>430796.00057672348</v>
       </c>
-      <c r="X9" s="23">
+      <c r="X9" s="17">
         <f t="shared" si="7"/>
         <v>4.1498794850559078</v>
       </c>
-      <c r="Y9" s="24">
+      <c r="Y9" s="18">
         <v>8.5</v>
       </c>
-      <c r="Z9" s="28">
+      <c r="Z9" s="22">
         <f t="shared" si="8"/>
         <v>1787751.4850374777</v>
       </c>
@@ -1768,7 +1768,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC9" s="29">
+      <c r="AC9" s="23">
         <f t="shared" si="2"/>
         <v>1787751.4850374777</v>
       </c>
@@ -1786,72 +1786,72 @@
         <v>1577.6976135063771</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="F10" s="18">
+      <c r="F10" s="12">
         <v>9</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="13">
         <v>13</v>
       </c>
-      <c r="H10" s="19">
-        <v>0</v>
-      </c>
-      <c r="I10" s="19">
-        <v>0</v>
-      </c>
-      <c r="J10" s="20">
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="14">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="12">
         <v>9</v>
       </c>
-      <c r="M10" s="19">
+      <c r="M10" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O10" s="19">
+      <c r="O10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P10" s="19">
+      <c r="P10" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="21">
+      <c r="Q10" s="15">
         <f t="shared" ref="Q10" si="11">+Q9+0.5</f>
         <v>9.25</v>
       </c>
-      <c r="R10" s="22">
+      <c r="R10" s="16">
         <v>9</v>
       </c>
-      <c r="S10" s="19">
+      <c r="S10" s="13">
         <f t="shared" si="6"/>
         <v>307484.10141549056</v>
       </c>
-      <c r="T10" s="19">
+      <c r="T10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U10" s="19">
+      <c r="U10" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V10" s="19">
+      <c r="V10" s="13">
         <f t="shared" si="1"/>
         <v>307484.10141549056</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="17">
         <f t="shared" si="7"/>
         <v>5.0418416693419372</v>
       </c>
-      <c r="Y10" s="24">
+      <c r="Y10" s="18">
         <v>9</v>
       </c>
-      <c r="Z10" s="28">
+      <c r="Z10" s="22">
         <f t="shared" si="8"/>
         <v>1550286.1551767825</v>
       </c>
@@ -1863,7 +1863,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC10" s="29">
+      <c r="AC10" s="23">
         <f t="shared" si="2"/>
         <v>1550286.1551767825</v>
       </c>
@@ -1881,71 +1881,71 @@
         <v>271.21825216101166</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="F11" s="18">
+      <c r="F11" s="12">
         <v>9.5</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="13">
         <v>12</v>
       </c>
-      <c r="H11" s="19">
-        <v>0</v>
-      </c>
-      <c r="I11" s="19">
-        <v>0</v>
-      </c>
-      <c r="J11" s="20">
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="14">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="12">
         <v>9.5</v>
       </c>
-      <c r="M11" s="19">
+      <c r="M11" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N11" s="19">
+      <c r="N11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O11" s="19">
+      <c r="O11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P11" s="19">
+      <c r="P11" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q11" s="21">
+      <c r="Q11" s="15">
         <v>9.75</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="16">
         <v>9.5</v>
       </c>
-      <c r="S11" s="19">
+      <c r="S11" s="13">
         <f t="shared" si="6"/>
         <v>45171.814017904799</v>
       </c>
-      <c r="T11" s="19">
+      <c r="T11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U11" s="19">
+      <c r="U11" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V11" s="19">
+      <c r="V11" s="13">
         <f t="shared" si="1"/>
         <v>45171.814017904799</v>
       </c>
-      <c r="X11" s="23">
+      <c r="X11" s="17">
         <f t="shared" si="7"/>
         <v>6.0613611314061915</v>
       </c>
-      <c r="Y11" s="24">
+      <c r="Y11" s="18">
         <v>9.5</v>
       </c>
-      <c r="Z11" s="28">
+      <c r="Z11" s="22">
         <f t="shared" si="8"/>
         <v>273802.67772323749</v>
       </c>
@@ -1957,7 +1957,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC11" s="29">
+      <c r="AC11" s="23">
         <f t="shared" si="2"/>
         <v>273802.67772323749</v>
       </c>
@@ -1975,72 +1975,72 @@
         <v>159.19010680325829</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="F12" s="18">
+      <c r="F12" s="12">
         <v>10</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="13">
         <v>11</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="13">
         <v>2</v>
       </c>
-      <c r="I12" s="19">
-        <v>0</v>
-      </c>
-      <c r="J12" s="20">
+      <c r="I12" s="13">
+        <v>0</v>
+      </c>
+      <c r="J12" s="14">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="12">
         <v>10</v>
       </c>
-      <c r="M12" s="19">
+      <c r="M12" s="13">
         <f t="shared" si="4"/>
         <v>0.84615384615384615</v>
       </c>
-      <c r="N12" s="19">
+      <c r="N12" s="13">
         <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P12" s="19">
+      <c r="P12" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q12" s="21">
+      <c r="Q12" s="15">
         <f t="shared" ref="Q12" si="12">+Q11+0.5</f>
         <v>10.25</v>
       </c>
-      <c r="R12" s="22">
+      <c r="R12" s="16">
         <v>10</v>
       </c>
-      <c r="S12" s="19">
+      <c r="S12" s="13">
         <f t="shared" si="6"/>
         <v>19323.140928221092</v>
       </c>
-      <c r="T12" s="19">
+      <c r="T12" s="13">
         <f t="shared" si="1"/>
         <v>3513.2983505856532</v>
       </c>
-      <c r="U12" s="19">
+      <c r="U12" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V12" s="19">
+      <c r="V12" s="13">
         <f t="shared" si="1"/>
         <v>22836.439278806745</v>
       </c>
-      <c r="X12" s="23">
+      <c r="X12" s="17">
         <f t="shared" si="7"/>
         <v>7.2185119744838255</v>
       </c>
-      <c r="Y12" s="24">
+      <c r="Y12" s="18">
         <v>10</v>
       </c>
-      <c r="Z12" s="28">
+      <c r="Z12" s="22">
         <f t="shared" si="8"/>
         <v>139484.32417500246</v>
       </c>
@@ -2052,7 +2052,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC12" s="29">
+      <c r="AC12" s="23">
         <f t="shared" si="2"/>
         <v>164845.11038863927</v>
       </c>
@@ -2070,71 +2070,71 @@
         <v>663.63088244525591</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="F13" s="18">
+      <c r="F13" s="12">
         <v>10.5</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="13">
         <v>8</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="13">
         <v>3</v>
       </c>
-      <c r="I13" s="19">
-        <v>0</v>
-      </c>
-      <c r="J13" s="20">
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="14">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="12">
         <v>10.5</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="13">
         <f t="shared" si="4"/>
         <v>0.72727272727272729</v>
       </c>
-      <c r="N13" s="19">
+      <c r="N13" s="13">
         <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P13" s="19">
+      <c r="P13" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q13" s="21">
+      <c r="Q13" s="15">
         <v>10.75</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="16">
         <v>10.5</v>
       </c>
-      <c r="S13" s="19">
+      <c r="S13" s="13">
         <f t="shared" si="6"/>
         <v>60060.444165349043</v>
       </c>
-      <c r="T13" s="19">
+      <c r="T13" s="13">
         <f t="shared" si="1"/>
         <v>22522.666562005888</v>
       </c>
-      <c r="U13" s="19">
+      <c r="U13" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V13" s="19">
+      <c r="V13" s="13">
         <f t="shared" si="1"/>
         <v>82583.110727354928</v>
       </c>
-      <c r="X13" s="23">
+      <c r="X13" s="17">
         <f t="shared" si="7"/>
         <v>8.5235861276697946</v>
       </c>
-      <c r="Y13" s="24">
+      <c r="Y13" s="18">
         <v>10.5</v>
       </c>
-      <c r="Z13" s="28">
+      <c r="Z13" s="22">
         <f t="shared" si="8"/>
         <v>511930.36870945536</v>
       </c>
@@ -2146,7 +2146,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC13" s="29">
+      <c r="AC13" s="23">
         <f t="shared" si="2"/>
         <v>703904.25697550108</v>
       </c>
@@ -2164,72 +2164,72 @@
         <v>1181.3210522571546</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="F14" s="18">
+      <c r="F14" s="12">
         <v>11</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="13">
         <v>5</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="13">
         <v>6</v>
       </c>
-      <c r="I14" s="19">
-        <v>0</v>
-      </c>
-      <c r="J14" s="20">
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="14">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="L14" s="18">
+      <c r="L14" s="12">
         <v>11</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="13">
         <f t="shared" si="4"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="N14" s="19">
+      <c r="N14" s="13">
         <f t="shared" si="0"/>
         <v>0.54545454545454541</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P14" s="19">
+      <c r="P14" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q14" s="21">
+      <c r="Q14" s="15">
         <f t="shared" ref="Q14" si="13">+Q13+0.5</f>
         <v>11.25</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="16">
         <v>11</v>
       </c>
-      <c r="S14" s="19">
+      <c r="S14" s="13">
         <f t="shared" si="6"/>
         <v>58340.473558908554</v>
       </c>
-      <c r="T14" s="19">
+      <c r="T14" s="13">
         <f t="shared" si="1"/>
         <v>70008.568270690259</v>
       </c>
-      <c r="U14" s="19">
+      <c r="U14" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V14" s="19">
+      <c r="V14" s="13">
         <f t="shared" si="1"/>
         <v>128349.04182959882</v>
       </c>
-      <c r="X14" s="23">
+      <c r="X14" s="17">
         <f t="shared" si="7"/>
         <v>9.9870868022135184</v>
       </c>
-      <c r="Y14" s="24">
+      <c r="Y14" s="18">
         <v>11</v>
       </c>
-      <c r="Z14" s="28">
+      <c r="Z14" s="22">
         <f t="shared" si="8"/>
         <v>582651.37351506238</v>
       </c>
@@ -2241,7 +2241,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC14" s="29">
+      <c r="AC14" s="23">
         <f t="shared" si="2"/>
         <v>1281833.0217331371</v>
       </c>
@@ -2259,71 +2259,71 @@
         <v>1788.6254399882125</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="F15" s="18">
+      <c r="F15" s="12">
         <v>11.5</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="13">
         <v>5</v>
       </c>
-      <c r="H15" s="19">
+      <c r="H15" s="13">
         <v>7</v>
       </c>
-      <c r="I15" s="19">
-        <v>0</v>
-      </c>
-      <c r="J15" s="20">
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="14">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="12">
         <v>11.5</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="13">
         <f t="shared" si="4"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="N15" s="19">
+      <c r="N15" s="13">
         <f t="shared" si="0"/>
         <v>0.58333333333333337</v>
       </c>
-      <c r="O15" s="19">
+      <c r="O15" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P15" s="19">
+      <c r="P15" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="15">
         <v>11.75</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="16">
         <v>11.5</v>
       </c>
-      <c r="S15" s="19">
+      <c r="S15" s="13">
         <f t="shared" si="6"/>
         <v>71114.19851134732</v>
       </c>
-      <c r="T15" s="19">
+      <c r="T15" s="13">
         <f t="shared" si="1"/>
         <v>99559.877915886245</v>
       </c>
-      <c r="U15" s="19">
+      <c r="U15" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V15" s="19">
+      <c r="V15" s="13">
         <f t="shared" si="1"/>
         <v>170674.07642723355</v>
       </c>
-      <c r="X15" s="23">
+      <c r="X15" s="17">
         <f t="shared" si="7"/>
         <v>11.619722450459651</v>
       </c>
-      <c r="Y15" s="24">
+      <c r="Y15" s="18">
         <v>11.5</v>
       </c>
-      <c r="Z15" s="28">
+      <c r="Z15" s="22">
         <f t="shared" si="8"/>
         <v>826327.24898874678</v>
       </c>
@@ -2335,7 +2335,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC15" s="29">
+      <c r="AC15" s="23">
         <f t="shared" si="2"/>
         <v>1983185.3975729921</v>
       </c>
@@ -2353,72 +2353,72 @@
         <v>1621.4509606898646</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="F16" s="18">
+      <c r="F16" s="12">
         <v>12</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="13">
         <v>3</v>
       </c>
-      <c r="H16" s="19">
+      <c r="H16" s="13">
         <v>10</v>
       </c>
-      <c r="I16" s="19">
-        <v>0</v>
-      </c>
-      <c r="J16" s="20">
+      <c r="I16" s="13">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="L16" s="18">
+      <c r="L16" s="12">
         <v>12</v>
       </c>
-      <c r="M16" s="19">
+      <c r="M16" s="13">
         <f>+IF($J16&gt;0,G16/$J16,0)</f>
         <v>0.23076923076923078</v>
       </c>
-      <c r="N16" s="19">
+      <c r="N16" s="13">
         <f t="shared" si="0"/>
         <v>0.76923076923076927</v>
       </c>
-      <c r="O16" s="19">
+      <c r="O16" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P16" s="19">
+      <c r="P16" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="Q16" s="15">
         <f t="shared" ref="Q16" si="14">+Q15+0.5</f>
         <v>12.25</v>
       </c>
-      <c r="R16" s="22">
+      <c r="R16" s="16">
         <v>12</v>
       </c>
-      <c r="S16" s="19">
+      <c r="S16" s="13">
         <f t="shared" si="6"/>
         <v>31528.482347668178</v>
       </c>
-      <c r="T16" s="19">
+      <c r="T16" s="13">
         <f t="shared" si="1"/>
         <v>105094.94115889393</v>
       </c>
-      <c r="U16" s="19">
+      <c r="U16" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V16" s="19">
+      <c r="V16" s="13">
         <f t="shared" si="1"/>
         <v>136623.4235065621</v>
       </c>
-      <c r="X16" s="23">
+      <c r="X16" s="17">
         <f t="shared" si="7"/>
         <v>13.432401167442283</v>
       </c>
-      <c r="Y16" s="24">
+      <c r="Y16" s="18">
         <v>12</v>
       </c>
-      <c r="Z16" s="28">
+      <c r="Z16" s="22">
         <f t="shared" si="8"/>
         <v>423503.22309450142</v>
       </c>
@@ -2430,7 +2430,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC16" s="29">
+      <c r="AC16" s="23">
         <f t="shared" si="2"/>
         <v>1835180.6334095062</v>
       </c>
@@ -2448,71 +2448,71 @@
         <v>834.85429343209762</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="F17" s="18">
+      <c r="F17" s="12">
         <v>12.5</v>
       </c>
-      <c r="G17" s="19">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19">
+      <c r="G17" s="13">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
         <v>3</v>
       </c>
-      <c r="I17" s="19">
-        <v>0</v>
-      </c>
-      <c r="J17" s="20">
+      <c r="I17" s="13">
+        <v>0</v>
+      </c>
+      <c r="J17" s="14">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="12">
         <v>12.5</v>
       </c>
-      <c r="M17" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="19">
+      <c r="M17" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P17" s="19">
+      <c r="P17" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q17" s="21">
+      <c r="Q17" s="15">
         <v>12.75</v>
       </c>
-      <c r="R17" s="22">
+      <c r="R17" s="16">
         <v>12.5</v>
       </c>
-      <c r="S17" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T17" s="19">
+      <c r="S17" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T17" s="13">
         <f t="shared" si="1"/>
         <v>62426.197021230109</v>
       </c>
-      <c r="U17" s="19">
+      <c r="U17" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V17" s="19">
+      <c r="V17" s="13">
         <f t="shared" si="1"/>
         <v>62426.197021230109</v>
       </c>
-      <c r="X17" s="23">
+      <c r="X17" s="17">
         <f t="shared" si="7"/>
         <v>15.436225484631182</v>
       </c>
-      <c r="Y17" s="24">
+      <c r="Y17" s="18">
         <v>12.5</v>
       </c>
-      <c r="Z17" s="28">
+      <c r="Z17" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2524,7 +2524,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC17" s="29">
+      <c r="AC17" s="23">
         <f t="shared" si="2"/>
         <v>963624.85336771933</v>
       </c>
@@ -2542,72 +2542,72 @@
         <v>340.52407930871288</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="F18" s="18">
+      <c r="F18" s="12">
         <v>13</v>
       </c>
-      <c r="G18" s="19">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19">
+      <c r="G18" s="13">
+        <v>0</v>
+      </c>
+      <c r="H18" s="13">
         <v>2</v>
       </c>
-      <c r="I18" s="19">
-        <v>0</v>
-      </c>
-      <c r="J18" s="20">
+      <c r="I18" s="13">
+        <v>0</v>
+      </c>
+      <c r="J18" s="14">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="12">
         <v>13</v>
       </c>
-      <c r="M18" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="19">
+      <c r="M18" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N18" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O18" s="19">
+      <c r="O18" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P18" s="19">
+      <c r="P18" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="Q18" s="15">
         <f t="shared" ref="Q18" si="15">+Q17+0.5</f>
         <v>13.25</v>
       </c>
-      <c r="R18" s="22">
+      <c r="R18" s="16">
         <v>13</v>
       </c>
-      <c r="S18" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T18" s="19">
+      <c r="S18" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T18" s="13">
         <f t="shared" si="1"/>
         <v>22700.435280447349</v>
       </c>
-      <c r="U18" s="19">
+      <c r="U18" s="13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V18" s="19">
+      <c r="V18" s="13">
         <f t="shared" si="1"/>
         <v>22700.435280447349</v>
       </c>
-      <c r="X18" s="23">
+      <c r="X18" s="17">
         <f t="shared" si="7"/>
         <v>17.642487512980097</v>
       </c>
-      <c r="Y18" s="24">
+      <c r="Y18" s="18">
         <v>13</v>
       </c>
-      <c r="Z18" s="28">
+      <c r="Z18" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2619,7 +2619,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC18" s="29">
+      <c r="AC18" s="23">
         <f t="shared" si="2"/>
         <v>400492.14597450517</v>
       </c>
@@ -2637,71 +2637,71 @@
         <v>95.084605900604544</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="F19" s="18">
+      <c r="F19" s="12">
         <v>13.5</v>
       </c>
-      <c r="G19" s="19">
-        <v>0</v>
-      </c>
-      <c r="H19" s="19">
-        <v>0</v>
-      </c>
-      <c r="I19" s="19">
-        <v>0</v>
-      </c>
-      <c r="J19" s="20">
+      <c r="G19" s="13">
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
+        <v>0</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0</v>
+      </c>
+      <c r="J19" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="12">
         <v>13.5</v>
       </c>
-      <c r="M19" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="21">
+      <c r="M19" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="15">
         <v>13.75</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="16">
         <v>13.5</v>
       </c>
-      <c r="S19" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U19" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V19" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X19" s="23">
+      <c r="S19" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V19" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X19" s="17">
         <f t="shared" si="7"/>
         <v>20.062664398656398</v>
       </c>
-      <c r="Y19" s="24">
+      <c r="Y19" s="18">
         <v>13.5</v>
       </c>
-      <c r="Z19" s="28">
+      <c r="Z19" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2713,7 +2713,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC19" s="29">
+      <c r="AC19" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2731,72 +2731,72 @@
         <v>0</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="F20" s="18">
+      <c r="F20" s="12">
         <v>14</v>
       </c>
-      <c r="G20" s="19">
-        <v>0</v>
-      </c>
-      <c r="H20" s="19">
-        <v>0</v>
-      </c>
-      <c r="I20" s="19">
-        <v>0</v>
-      </c>
-      <c r="J20" s="20">
+      <c r="G20" s="13">
+        <v>0</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
+        <v>0</v>
+      </c>
+      <c r="J20" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="12">
         <v>14</v>
       </c>
-      <c r="M20" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P20" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q20" s="21">
+      <c r="M20" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N20" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="15">
         <f t="shared" ref="Q20" si="16">+Q19+0.5</f>
         <v>14.25</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="16">
         <v>14</v>
       </c>
-      <c r="S20" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U20" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V20" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X20" s="23">
+      <c r="S20" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U20" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V20" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X20" s="17">
         <f t="shared" si="7"/>
         <v>22.708414059946083</v>
       </c>
-      <c r="Y20" s="24">
+      <c r="Y20" s="18">
         <v>14</v>
       </c>
-      <c r="Z20" s="28">
+      <c r="Z20" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2808,7 +2808,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC20" s="29">
+      <c r="AC20" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2826,71 +2826,71 @@
         <v>0</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="F21" s="18">
+      <c r="F21" s="12">
         <v>14.5</v>
       </c>
-      <c r="G21" s="19">
-        <v>0</v>
-      </c>
-      <c r="H21" s="19">
-        <v>0</v>
-      </c>
-      <c r="I21" s="19">
-        <v>0</v>
-      </c>
-      <c r="J21" s="20">
+      <c r="G21" s="13">
+        <v>0</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0</v>
+      </c>
+      <c r="J21" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L21" s="18">
+      <c r="L21" s="12">
         <v>14.5</v>
       </c>
-      <c r="M21" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P21" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="21">
+      <c r="M21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="15">
         <v>14.75</v>
       </c>
-      <c r="R21" s="22">
+      <c r="R21" s="16">
         <v>14.5</v>
       </c>
-      <c r="S21" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T21" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U21" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V21" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X21" s="23">
+      <c r="S21" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T21" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U21" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X21" s="17">
         <f t="shared" si="7"/>
         <v>25.591571178065511</v>
       </c>
-      <c r="Y21" s="24">
+      <c r="Y21" s="18">
         <v>14.5</v>
       </c>
-      <c r="Z21" s="28">
+      <c r="Z21" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2902,7 +2902,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC21" s="29">
+      <c r="AC21" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2920,72 +2920,72 @@
         <v>259.04554587112688</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="F22" s="18">
+      <c r="F22" s="12">
         <v>15</v>
       </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-      <c r="H22" s="19">
+      <c r="G22" s="13">
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
         <v>2</v>
       </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="20">
+      <c r="I22" s="13">
+        <v>0</v>
+      </c>
+      <c r="J22" s="14">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L22" s="18">
+      <c r="L22" s="12">
         <v>15</v>
       </c>
-      <c r="M22" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N22" s="19">
+      <c r="M22" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="O22" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P22" s="19">
+      <c r="O22" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="13">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="Q22" s="21">
+      <c r="Q22" s="15">
         <f t="shared" ref="Q22" si="17">+Q21+0.5</f>
         <v>15.25</v>
       </c>
-      <c r="R22" s="22">
+      <c r="R22" s="16">
         <v>15</v>
       </c>
-      <c r="S22" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T22" s="19">
+      <c r="S22" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="13">
         <f t="shared" si="6"/>
         <v>11350.217640223675</v>
       </c>
-      <c r="U22" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V22" s="19">
+      <c r="U22" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V22" s="13">
         <f t="shared" si="6"/>
         <v>11350.217640223675</v>
       </c>
-      <c r="X22" s="23">
+      <c r="X22" s="17">
         <f t="shared" si="7"/>
         <v>28.724143418143864</v>
       </c>
-      <c r="Y22" s="24">
+      <c r="Y22" s="18">
         <v>15</v>
       </c>
-      <c r="Z22" s="28">
+      <c r="Z22" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -2997,7 +2997,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC22" s="29">
+      <c r="AC22" s="23">
         <f t="shared" si="8"/>
         <v>326025.27932493127</v>
       </c>
@@ -3015,71 +3015,71 @@
         <v>0</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="F23" s="18">
+      <c r="F23" s="12">
         <v>15.5</v>
       </c>
-      <c r="G23" s="19">
-        <v>0</v>
-      </c>
-      <c r="H23" s="19">
-        <v>0</v>
-      </c>
-      <c r="I23" s="19">
-        <v>0</v>
-      </c>
-      <c r="J23" s="20">
+      <c r="G23" s="13">
+        <v>0</v>
+      </c>
+      <c r="H23" s="13">
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
+        <v>0</v>
+      </c>
+      <c r="J23" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L23" s="18">
+      <c r="L23" s="12">
         <v>15.5</v>
       </c>
-      <c r="M23" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P23" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="21">
+      <c r="M23" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N23" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="15">
         <v>15.75</v>
       </c>
-      <c r="R23" s="22">
+      <c r="R23" s="16">
         <v>15.5</v>
       </c>
-      <c r="S23" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T23" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U23" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V23" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X23" s="23">
+      <c r="S23" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T23" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V23" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X23" s="17">
         <f t="shared" si="7"/>
         <v>32.118307859609843</v>
       </c>
-      <c r="Y23" s="24">
+      <c r="Y23" s="18">
         <v>15.5</v>
       </c>
-      <c r="Z23" s="28">
+      <c r="Z23" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3091,7 +3091,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC23" s="29">
+      <c r="AC23" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3109,72 +3109,72 @@
         <v>0</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="F24" s="18">
+      <c r="F24" s="12">
         <v>16</v>
       </c>
-      <c r="G24" s="19">
-        <v>0</v>
-      </c>
-      <c r="H24" s="19">
-        <v>0</v>
-      </c>
-      <c r="I24" s="19">
-        <v>0</v>
-      </c>
-      <c r="J24" s="20">
+      <c r="G24" s="13">
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <v>0</v>
+      </c>
+      <c r="I24" s="13">
+        <v>0</v>
+      </c>
+      <c r="J24" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L24" s="18">
+      <c r="L24" s="12">
         <v>16</v>
       </c>
-      <c r="M24" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N24" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O24" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P24" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q24" s="21">
+      <c r="M24" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O24" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="15">
         <f t="shared" ref="Q24" si="18">+Q23+0.5</f>
         <v>16.25</v>
       </c>
-      <c r="R24" s="22">
+      <c r="R24" s="16">
         <v>16</v>
       </c>
-      <c r="S24" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T24" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U24" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V24" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X24" s="23">
+      <c r="S24" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T24" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U24" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X24" s="17">
         <f t="shared" si="7"/>
         <v>35.786407617725658</v>
       </c>
-      <c r="Y24" s="24">
+      <c r="Y24" s="18">
         <v>16</v>
       </c>
-      <c r="Z24" s="28">
+      <c r="Z24" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3186,7 +3186,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC24" s="29">
+      <c r="AC24" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3204,71 +3204,71 @@
         <v>0</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="F25" s="18">
+      <c r="F25" s="12">
         <v>16.5</v>
       </c>
-      <c r="G25" s="19">
-        <v>0</v>
-      </c>
-      <c r="H25" s="19">
-        <v>0</v>
-      </c>
-      <c r="I25" s="19">
-        <v>0</v>
-      </c>
-      <c r="J25" s="20">
+      <c r="G25" s="13">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0</v>
+      </c>
+      <c r="J25" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L25" s="18">
+      <c r="L25" s="12">
         <v>16.5</v>
       </c>
-      <c r="M25" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P25" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q25" s="21">
+      <c r="M25" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="15">
         <v>16.75</v>
       </c>
-      <c r="R25" s="22">
+      <c r="R25" s="16">
         <v>16.5</v>
       </c>
-      <c r="S25" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T25" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U25" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V25" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X25" s="23">
+      <c r="S25" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V25" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X25" s="17">
         <f t="shared" si="7"/>
         <v>39.740948640144921</v>
       </c>
-      <c r="Y25" s="24">
+      <c r="Y25" s="18">
         <v>16.5</v>
       </c>
-      <c r="Z25" s="28">
+      <c r="Z25" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3280,7 +3280,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC25" s="29">
+      <c r="AC25" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3298,72 +3298,72 @@
         <v>0</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="F26" s="18">
+      <c r="F26" s="12">
         <v>17</v>
       </c>
-      <c r="G26" s="19">
-        <v>0</v>
-      </c>
-      <c r="H26" s="19">
-        <v>0</v>
-      </c>
-      <c r="I26" s="19">
-        <v>0</v>
-      </c>
-      <c r="J26" s="20">
+      <c r="G26" s="13">
+        <v>0</v>
+      </c>
+      <c r="H26" s="13">
+        <v>0</v>
+      </c>
+      <c r="I26" s="13">
+        <v>0</v>
+      </c>
+      <c r="J26" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L26" s="18">
+      <c r="L26" s="12">
         <v>17</v>
       </c>
-      <c r="M26" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N26" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O26" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P26" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="21">
+      <c r="M26" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O26" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="15">
         <f t="shared" ref="Q26" si="19">+Q25+0.5</f>
         <v>17.25</v>
       </c>
-      <c r="R26" s="22">
+      <c r="R26" s="16">
         <v>17</v>
       </c>
-      <c r="S26" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T26" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U26" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V26" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X26" s="23">
+      <c r="S26" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X26" s="17">
         <f t="shared" si="7"/>
         <v>43.994596664199015</v>
       </c>
-      <c r="Y26" s="24">
+      <c r="Y26" s="18">
         <v>17</v>
       </c>
-      <c r="Z26" s="28">
+      <c r="Z26" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3375,7 +3375,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC26" s="29">
+      <c r="AC26" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3393,71 +3393,71 @@
         <v>0</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="F27" s="18">
+      <c r="F27" s="12">
         <v>17.5</v>
       </c>
-      <c r="G27" s="19">
-        <v>0</v>
-      </c>
-      <c r="H27" s="19">
-        <v>0</v>
-      </c>
-      <c r="I27" s="19">
-        <v>0</v>
-      </c>
-      <c r="J27" s="20">
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
+        <v>0</v>
+      </c>
+      <c r="J27" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L27" s="18">
+      <c r="L27" s="12">
         <v>17.5</v>
       </c>
-      <c r="M27" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N27" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O27" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P27" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q27" s="21">
+      <c r="M27" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="15">
         <v>17.75</v>
       </c>
-      <c r="R27" s="22">
+      <c r="R27" s="16">
         <v>17.5</v>
       </c>
-      <c r="S27" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T27" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U27" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V27" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X27" s="23">
+      <c r="S27" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X27" s="17">
         <f t="shared" si="7"/>
         <v>48.560174322182647</v>
       </c>
-      <c r="Y27" s="24">
+      <c r="Y27" s="18">
         <v>17.5</v>
       </c>
-      <c r="Z27" s="28">
+      <c r="Z27" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3469,7 +3469,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC27" s="29">
+      <c r="AC27" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3486,72 +3486,72 @@
         <f>Alg!C28+Cad!C28</f>
         <v>0</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F28" s="12">
         <v>18</v>
       </c>
-      <c r="G28" s="19">
-        <v>0</v>
-      </c>
-      <c r="H28" s="19">
-        <v>0</v>
-      </c>
-      <c r="I28" s="19">
-        <v>0</v>
-      </c>
-      <c r="J28" s="20">
+      <c r="G28" s="13">
+        <v>0</v>
+      </c>
+      <c r="H28" s="13">
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
+        <v>0</v>
+      </c>
+      <c r="J28" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L28" s="18">
+      <c r="L28" s="12">
         <v>18</v>
       </c>
-      <c r="M28" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N28" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O28" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P28" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q28" s="21">
+      <c r="M28" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="15">
         <f t="shared" ref="Q28" si="20">+Q27+0.5</f>
         <v>18.25</v>
       </c>
-      <c r="R28" s="22">
+      <c r="R28" s="16">
         <v>18</v>
       </c>
-      <c r="S28" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T28" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U28" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V28" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X28" s="23">
+      <c r="S28" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U28" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X28" s="17">
         <f t="shared" si="7"/>
         <v>53.450658383266735</v>
       </c>
-      <c r="Y28" s="24">
+      <c r="Y28" s="18">
         <v>18</v>
       </c>
-      <c r="Z28" s="28">
+      <c r="Z28" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3563,7 +3563,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC28" s="29">
+      <c r="AC28" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3580,71 +3580,71 @@
         <f>Alg!C29+Cad!C29</f>
         <v>0</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="12">
         <v>18.5</v>
       </c>
-      <c r="G29" s="19">
-        <v>0</v>
-      </c>
-      <c r="H29" s="19">
-        <v>0</v>
-      </c>
-      <c r="I29" s="19">
-        <v>0</v>
-      </c>
-      <c r="J29" s="20">
+      <c r="G29" s="13">
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <v>0</v>
+      </c>
+      <c r="I29" s="13">
+        <v>0</v>
+      </c>
+      <c r="J29" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L29" s="18">
+      <c r="L29" s="12">
         <v>18.5</v>
       </c>
-      <c r="M29" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N29" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O29" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P29" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q29" s="21">
+      <c r="M29" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="15">
         <v>18.75</v>
       </c>
-      <c r="R29" s="22">
+      <c r="R29" s="16">
         <v>18.5</v>
       </c>
-      <c r="S29" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T29" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U29" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V29" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X29" s="23">
+      <c r="S29" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U29" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V29" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X29" s="17">
         <f t="shared" si="7"/>
         <v>58.679177121843765</v>
       </c>
-      <c r="Y29" s="24">
+      <c r="Y29" s="18">
         <v>18.5</v>
       </c>
-      <c r="Z29" s="28">
+      <c r="Z29" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3656,7 +3656,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC29" s="29">
+      <c r="AC29" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3673,72 +3673,72 @@
         <f>Alg!C30+Cad!C30</f>
         <v>0</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="12">
         <v>19</v>
       </c>
-      <c r="G30" s="19">
-        <v>0</v>
-      </c>
-      <c r="H30" s="19">
-        <v>0</v>
-      </c>
-      <c r="I30" s="19">
-        <v>0</v>
-      </c>
-      <c r="J30" s="20">
+      <c r="G30" s="13">
+        <v>0</v>
+      </c>
+      <c r="H30" s="13">
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
+        <v>0</v>
+      </c>
+      <c r="J30" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L30" s="18">
+      <c r="L30" s="12">
         <v>19</v>
       </c>
-      <c r="M30" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N30" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O30" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P30" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="21">
+      <c r="M30" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O30" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="15">
         <f t="shared" ref="Q30" si="21">+Q29+0.5</f>
         <v>19.25</v>
       </c>
-      <c r="R30" s="22">
+      <c r="R30" s="16">
         <v>19</v>
       </c>
-      <c r="S30" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T30" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U30" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V30" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X30" s="23">
+      <c r="S30" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T30" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U30" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X30" s="17">
         <f t="shared" si="7"/>
         <v>64.259007803132704</v>
       </c>
-      <c r="Y30" s="24">
+      <c r="Y30" s="18">
         <v>19</v>
       </c>
-      <c r="Z30" s="28">
+      <c r="Z30" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3750,7 +3750,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC30" s="29">
+      <c r="AC30" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3767,71 +3767,71 @@
         <f>Alg!C31+Cad!C31</f>
         <v>0</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="12">
         <v>19.5</v>
       </c>
-      <c r="G31" s="19">
-        <v>0</v>
-      </c>
-      <c r="H31" s="19">
-        <v>0</v>
-      </c>
-      <c r="I31" s="19">
-        <v>0</v>
-      </c>
-      <c r="J31" s="20">
+      <c r="G31" s="13">
+        <v>0</v>
+      </c>
+      <c r="H31" s="13">
+        <v>0</v>
+      </c>
+      <c r="I31" s="13">
+        <v>0</v>
+      </c>
+      <c r="J31" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L31" s="18">
+      <c r="L31" s="12">
         <v>19.5</v>
       </c>
-      <c r="M31" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N31" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O31" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P31" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q31" s="21">
+      <c r="M31" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O31" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="15">
         <v>19.75</v>
       </c>
-      <c r="R31" s="22">
+      <c r="R31" s="16">
         <v>19.5</v>
       </c>
-      <c r="S31" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T31" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U31" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V31" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X31" s="23">
+      <c r="S31" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U31" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V31" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X31" s="17">
         <f t="shared" si="7"/>
         <v>70.203574277770713</v>
       </c>
-      <c r="Y31" s="24">
+      <c r="Y31" s="18">
         <v>19.5</v>
       </c>
-      <c r="Z31" s="28">
+      <c r="Z31" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3843,7 +3843,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC31" s="29">
+      <c r="AC31" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3860,72 +3860,72 @@
         <f>Alg!C32+Cad!C32</f>
         <v>0</v>
       </c>
-      <c r="F32" s="18">
+      <c r="F32" s="12">
         <v>20</v>
       </c>
-      <c r="G32" s="19">
-        <v>0</v>
-      </c>
-      <c r="H32" s="19">
-        <v>0</v>
-      </c>
-      <c r="I32" s="19">
-        <v>0</v>
-      </c>
-      <c r="J32" s="20">
+      <c r="G32" s="13">
+        <v>0</v>
+      </c>
+      <c r="H32" s="13">
+        <v>0</v>
+      </c>
+      <c r="I32" s="13">
+        <v>0</v>
+      </c>
+      <c r="J32" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L32" s="18">
+      <c r="L32" s="12">
         <v>20</v>
       </c>
-      <c r="M32" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N32" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O32" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P32" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="21">
+      <c r="M32" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N32" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O32" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="15">
         <f t="shared" ref="Q32" si="22">+Q31+0.5</f>
         <v>20.25</v>
       </c>
-      <c r="R32" s="22">
+      <c r="R32" s="16">
         <v>20</v>
       </c>
-      <c r="S32" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T32" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U32" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V32" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X32" s="23">
+      <c r="S32" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T32" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U32" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V32" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X32" s="17">
         <f t="shared" si="7"/>
         <v>76.526444677905573</v>
       </c>
-      <c r="Y32" s="24">
+      <c r="Y32" s="18">
         <v>20</v>
       </c>
-      <c r="Z32" s="28">
+      <c r="Z32" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3937,7 +3937,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC32" s="29">
+      <c r="AC32" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3954,71 +3954,71 @@
         <f>Alg!C33+Cad!C33</f>
         <v>0</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="12">
         <v>20.5</v>
       </c>
-      <c r="G33" s="19">
-        <v>0</v>
-      </c>
-      <c r="H33" s="19">
-        <v>0</v>
-      </c>
-      <c r="I33" s="19">
-        <v>0</v>
-      </c>
-      <c r="J33" s="20">
+      <c r="G33" s="13">
+        <v>0</v>
+      </c>
+      <c r="H33" s="13">
+        <v>0</v>
+      </c>
+      <c r="I33" s="13">
+        <v>0</v>
+      </c>
+      <c r="J33" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L33" s="18">
+      <c r="L33" s="12">
         <v>20.5</v>
       </c>
-      <c r="M33" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N33" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O33" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P33" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q33" s="21">
+      <c r="M33" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N33" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O33" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q33" s="15">
         <v>20.75</v>
       </c>
-      <c r="R33" s="22">
+      <c r="R33" s="16">
         <v>20.5</v>
       </c>
-      <c r="S33" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T33" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U33" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V33" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X33" s="23">
+      <c r="S33" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T33" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U33" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V33" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X33" s="17">
         <f t="shared" si="7"/>
         <v>83.241329207995491</v>
       </c>
-      <c r="Y33" s="24">
+      <c r="Y33" s="18">
         <v>20.5</v>
       </c>
-      <c r="Z33" s="28">
+      <c r="Z33" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4030,7 +4030,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC33" s="29">
+      <c r="AC33" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4047,72 +4047,72 @@
         <f>Alg!C34+Cad!C34</f>
         <v>0</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="12">
         <v>21</v>
       </c>
-      <c r="G34" s="19">
-        <v>0</v>
-      </c>
-      <c r="H34" s="19">
-        <v>0</v>
-      </c>
-      <c r="I34" s="19">
-        <v>0</v>
-      </c>
-      <c r="J34" s="20">
+      <c r="G34" s="13">
+        <v>0</v>
+      </c>
+      <c r="H34" s="13">
+        <v>0</v>
+      </c>
+      <c r="I34" s="13">
+        <v>0</v>
+      </c>
+      <c r="J34" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L34" s="18">
+      <c r="L34" s="12">
         <v>21</v>
       </c>
-      <c r="M34" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N34" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O34" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P34" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q34" s="21">
+      <c r="M34" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N34" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O34" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="15">
         <f t="shared" ref="Q34" si="23">+Q33+0.5</f>
         <v>21.25</v>
       </c>
-      <c r="R34" s="22">
+      <c r="R34" s="16">
         <v>21</v>
       </c>
-      <c r="S34" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T34" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U34" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V34" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X34" s="23">
+      <c r="S34" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T34" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U34" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V34" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X34" s="17">
         <f t="shared" si="7"/>
         <v>90.362078024138555</v>
       </c>
-      <c r="Y34" s="24">
+      <c r="Y34" s="18">
         <v>21</v>
       </c>
-      <c r="Z34" s="28">
+      <c r="Z34" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4124,7 +4124,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC34" s="29">
+      <c r="AC34" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4141,68 +4141,68 @@
         <f>Alg!C35+Cad!C35</f>
         <v>0</v>
       </c>
-      <c r="F35" s="18">
+      <c r="F35" s="12">
         <v>21.5</v>
       </c>
-      <c r="G35" s="19">
-        <v>0</v>
-      </c>
-      <c r="H35" s="19">
-        <v>0</v>
-      </c>
-      <c r="I35" s="19">
-        <v>0</v>
-      </c>
-      <c r="J35" s="20">
+      <c r="G35" s="13">
+        <v>0</v>
+      </c>
+      <c r="H35" s="13">
+        <v>0</v>
+      </c>
+      <c r="I35" s="13">
+        <v>0</v>
+      </c>
+      <c r="J35" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L35" s="18">
+      <c r="L35" s="12">
         <v>21.5</v>
       </c>
-      <c r="M35" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O35" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P35" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R35" s="22">
+      <c r="M35" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R35" s="16">
         <v>21.5</v>
       </c>
-      <c r="S35" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T35" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U35" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V35" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X35" s="23">
+      <c r="S35" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T35" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U35" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V35" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X35" s="17">
         <f t="shared" si="7"/>
         <v>97.902679196300895</v>
       </c>
-      <c r="Y35" s="24">
+      <c r="Y35" s="18">
         <v>21.5</v>
       </c>
-      <c r="Z35" s="28">
+      <c r="Z35" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4214,7 +4214,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC35" s="29">
+      <c r="AC35" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4231,68 +4231,68 @@
         <f>Alg!C36+Cad!C36</f>
         <v>0</v>
       </c>
-      <c r="F36" s="18">
+      <c r="F36" s="12">
         <v>22</v>
       </c>
-      <c r="G36" s="19">
-        <v>0</v>
-      </c>
-      <c r="H36" s="19">
-        <v>0</v>
-      </c>
-      <c r="I36" s="19">
-        <v>0</v>
-      </c>
-      <c r="J36" s="20">
+      <c r="G36" s="13">
+        <v>0</v>
+      </c>
+      <c r="H36" s="13">
+        <v>0</v>
+      </c>
+      <c r="I36" s="13">
+        <v>0</v>
+      </c>
+      <c r="J36" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L36" s="18">
+      <c r="L36" s="12">
         <v>22</v>
       </c>
-      <c r="M36" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N36" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O36" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P36" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R36" s="22">
+      <c r="M36" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N36" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O36" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R36" s="16">
         <v>22</v>
       </c>
-      <c r="S36" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T36" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U36" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V36" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X36" s="23">
+      <c r="S36" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T36" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U36" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V36" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X36" s="17">
         <f t="shared" si="7"/>
         <v>105.8772567482907</v>
       </c>
-      <c r="Y36" s="24">
+      <c r="Y36" s="18">
         <v>22</v>
       </c>
-      <c r="Z36" s="28">
+      <c r="Z36" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4304,7 +4304,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC36" s="29">
+      <c r="AC36" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4321,68 +4321,68 @@
         <f>Alg!C37+Cad!C37</f>
         <v>0</v>
       </c>
-      <c r="F37" s="18">
+      <c r="F37" s="12">
         <v>22.5</v>
       </c>
-      <c r="G37" s="19">
-        <v>0</v>
-      </c>
-      <c r="H37" s="19">
-        <v>0</v>
-      </c>
-      <c r="I37" s="19">
-        <v>0</v>
-      </c>
-      <c r="J37" s="20">
+      <c r="G37" s="13">
+        <v>0</v>
+      </c>
+      <c r="H37" s="13">
+        <v>0</v>
+      </c>
+      <c r="I37" s="13">
+        <v>0</v>
+      </c>
+      <c r="J37" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L37" s="18">
+      <c r="L37" s="12">
         <v>22.5</v>
       </c>
-      <c r="M37" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N37" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O37" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R37" s="22">
+      <c r="M37" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N37" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O37" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R37" s="16">
         <v>22.5</v>
       </c>
-      <c r="S37" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T37" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U37" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V37" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X37" s="23">
+      <c r="S37" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T37" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U37" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V37" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X37" s="17">
         <f t="shared" si="7"/>
         <v>114.30006877076555</v>
       </c>
-      <c r="Y37" s="24">
+      <c r="Y37" s="18">
         <v>22.5</v>
       </c>
-      <c r="Z37" s="28">
+      <c r="Z37" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4394,7 +4394,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC37" s="29">
+      <c r="AC37" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4411,68 +4411,68 @@
         <f>Alg!C38+Cad!C38</f>
         <v>0</v>
       </c>
-      <c r="F38" s="18">
+      <c r="F38" s="12">
         <v>23</v>
       </c>
-      <c r="G38" s="19">
-        <v>0</v>
-      </c>
-      <c r="H38" s="19">
-        <v>0</v>
-      </c>
-      <c r="I38" s="19">
-        <v>0</v>
-      </c>
-      <c r="J38" s="20">
+      <c r="G38" s="13">
+        <v>0</v>
+      </c>
+      <c r="H38" s="13">
+        <v>0</v>
+      </c>
+      <c r="I38" s="13">
+        <v>0</v>
+      </c>
+      <c r="J38" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L38" s="18">
+      <c r="L38" s="12">
         <v>23</v>
       </c>
-      <c r="M38" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N38" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O38" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P38" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R38" s="22">
+      <c r="M38" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N38" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O38" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R38" s="16">
         <v>23</v>
       </c>
-      <c r="S38" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T38" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U38" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V38" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X38" s="23">
+      <c r="S38" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T38" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U38" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V38" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X38" s="17">
         <f t="shared" si="7"/>
         <v>123.18550560294707</v>
       </c>
-      <c r="Y38" s="24">
+      <c r="Y38" s="18">
         <v>23</v>
       </c>
-      <c r="Z38" s="28">
+      <c r="Z38" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4484,7 +4484,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC38" s="29">
+      <c r="AC38" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4500,68 +4500,68 @@
       <c r="C39">
         <v>0</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="12">
         <v>23.5</v>
       </c>
-      <c r="G39" s="19">
-        <v>0</v>
-      </c>
-      <c r="H39" s="19">
-        <v>0</v>
-      </c>
-      <c r="I39" s="19">
-        <v>0</v>
-      </c>
-      <c r="J39" s="20">
+      <c r="G39" s="13">
+        <v>0</v>
+      </c>
+      <c r="H39" s="13">
+        <v>0</v>
+      </c>
+      <c r="I39" s="13">
+        <v>0</v>
+      </c>
+      <c r="J39" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L39" s="18">
+      <c r="L39" s="12">
         <v>23.5</v>
       </c>
-      <c r="M39" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N39" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O39" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R39" s="22">
+      <c r="M39" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N39" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O39" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R39" s="16">
         <v>23.5</v>
       </c>
-      <c r="S39" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T39" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U39" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V39" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X39" s="23">
+      <c r="S39" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T39" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U39" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V39" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X39" s="17">
         <f t="shared" si="7"/>
         <v>132.54808807905391</v>
       </c>
-      <c r="Y39" s="24">
+      <c r="Y39" s="18">
         <v>23.5</v>
       </c>
-      <c r="Z39" s="28">
+      <c r="Z39" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4573,7 +4573,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC39" s="29">
+      <c r="AC39" s="23">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4589,80 +4589,80 @@
       <c r="C40">
         <v>0</v>
       </c>
-      <c r="F40" s="30">
+      <c r="F40" s="24">
         <v>24</v>
       </c>
-      <c r="G40" s="19">
-        <v>0</v>
-      </c>
-      <c r="H40" s="19">
-        <v>0</v>
-      </c>
-      <c r="I40" s="19">
-        <v>0</v>
-      </c>
-      <c r="J40" s="31">
+      <c r="G40" s="13">
+        <v>0</v>
+      </c>
+      <c r="H40" s="13">
+        <v>0</v>
+      </c>
+      <c r="I40" s="13">
+        <v>0</v>
+      </c>
+      <c r="J40" s="25">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L40" s="30">
+      <c r="L40" s="24">
         <v>24</v>
       </c>
-      <c r="M40" s="32">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="N40" s="32">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O40" s="32">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P40" s="32">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R40" s="33">
+      <c r="M40" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="N40" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="O40" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R40" s="27">
         <v>24</v>
       </c>
-      <c r="S40" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="T40" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="U40" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="V40" s="32">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="X40" s="23">
+      <c r="S40" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T40" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U40" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="26">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X40" s="17">
         <f t="shared" si="7"/>
         <v>142.40246583579469</v>
       </c>
-      <c r="Y40" s="34">
+      <c r="Y40" s="28">
         <v>24</v>
       </c>
-      <c r="Z40" s="35">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AA40" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AB40" s="36">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="AC40" s="37">
+      <c r="Z40" s="29">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AA40" s="30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="30">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AC40" s="31">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4678,92 +4678,92 @@
       <c r="C41">
         <v>0</v>
       </c>
-      <c r="F41" s="38" t="s">
+      <c r="F41" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G41" s="39">
+      <c r="G41" s="33">
         <f>+SUM(G3:G40)</f>
         <v>94</v>
       </c>
-      <c r="H41" s="39">
+      <c r="H41" s="33">
         <f t="shared" ref="H41:I41" si="24">+SUM(H3:H40)</f>
         <v>35</v>
       </c>
-      <c r="I41" s="39">
+      <c r="I41" s="33">
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="J41" s="40">
+      <c r="J41" s="34">
         <f>+SUM(J3:J40)</f>
         <v>129</v>
       </c>
-      <c r="L41" s="38" t="s">
+      <c r="L41" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M41" s="41">
+      <c r="M41" s="35">
         <f t="shared" si="4"/>
         <v>0.72868217054263562</v>
       </c>
-      <c r="N41" s="41">
+      <c r="N41" s="35">
         <f t="shared" si="4"/>
         <v>0.27131782945736432</v>
       </c>
-      <c r="O41" s="41">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P41" s="42">
+      <c r="O41" s="35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="36">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="R41" s="43" t="s">
+      <c r="R41" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="S41" s="44">
+      <c r="S41" s="38">
         <f>+SUM(S3:S40)</f>
         <v>1565165.0611131531</v>
       </c>
-      <c r="T41" s="44">
+      <c r="T41" s="38">
         <f t="shared" ref="T41:U41" si="25">+SUM(T3:T40)</f>
         <v>397176.20219996315</v>
       </c>
-      <c r="U41" s="44">
+      <c r="U41" s="38">
         <f t="shared" si="25"/>
         <v>0</v>
       </c>
-      <c r="V41" s="45">
+      <c r="V41" s="39">
         <f>+SUM(V3:V40)</f>
         <v>1962341.2633131163</v>
       </c>
-      <c r="W41" s="46">
+      <c r="W41" s="40">
         <f>+B44</f>
         <v>1968016.372133228</v>
       </c>
-      <c r="X41" s="47"/>
-      <c r="Y41" s="48" t="s">
+      <c r="X41" s="41"/>
+      <c r="Y41" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="Z41" s="49">
+      <c r="Z41" s="43">
         <f>+SUM(Z3:Z40)</f>
         <v>7771805.8397358339</v>
       </c>
-      <c r="AA41" s="49">
+      <c r="AA41" s="43">
         <f t="shared" ref="AA41:AC41" si="26">+SUM(AA3:AA40)</f>
         <v>5175194.1602641623</v>
       </c>
-      <c r="AB41" s="49">
+      <c r="AB41" s="43">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AC41" s="49">
+      <c r="AC41" s="43">
         <f t="shared" si="26"/>
         <v>12946999.999999998</v>
       </c>
-      <c r="AD41" s="50">
+      <c r="AD41" s="44">
         <f>+C44</f>
         <v>12497.20493776615</v>
       </c>
-      <c r="AE41" s="49">
+      <c r="AE41" s="43">
         <f>+AC41/1000</f>
         <v>12946.999999999998</v>
       </c>
@@ -4779,42 +4779,41 @@
       <c r="C42">
         <v>0</v>
       </c>
-      <c r="R42" s="51" t="s">
+      <c r="R42" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="S42" s="52">
+      <c r="S42" s="46">
         <f>SUMPRODUCT(S3:S40, $R$3:$R$40)/S41</f>
         <v>8.7742404051207235</v>
       </c>
-      <c r="T42" s="52">
+      <c r="T42" s="46">
         <f>SUMPRODUCT(T3:T40, $R$3:$R$40)/T41</f>
         <v>11.817121678844916</v>
       </c>
-      <c r="U42" s="52" t="e">
-        <f t="shared" ref="U42:V42" si="27">SUMPRODUCT(U3:U40, $R$3:$R$40)/U41</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V42" s="52">
-        <f t="shared" si="27"/>
+      <c r="U42" s="46">
+        <v>0</v>
+      </c>
+      <c r="V42" s="46">
+        <f t="shared" ref="U42:V42" si="27">SUMPRODUCT(V3:V40, $R$3:$R$40)/V41</f>
         <v>9.3901169861404234</v>
       </c>
-      <c r="X42" s="47"/>
-      <c r="Y42" s="53" t="s">
+      <c r="X42" s="41"/>
+      <c r="Y42" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="Z42" s="54">
+      <c r="Z42" s="48">
         <f>IF(S41&gt;0,Z41/S41,0)</f>
         <v>4.965486409598542</v>
       </c>
-      <c r="AA42" s="54">
+      <c r="AA42" s="48">
         <f t="shared" ref="AA42:AC42" si="28">IF(T41&gt;0,AA41/T41,0)</f>
         <v>13.029970405071371</v>
       </c>
-      <c r="AB42" s="54">
+      <c r="AB42" s="48">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AC42" s="54">
+      <c r="AC42" s="48">
         <f t="shared" si="28"/>
         <v>6.5977311092877633</v>
       </c>

</xml_diff>